<commit_message>
screenshots and video updated
</commit_message>
<xml_diff>
--- a/documents/Promotion.xlsx
+++ b/documents/Promotion.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\enginkirmaci\SnapIt\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DFD5AD-BD19-4091-9F0E-7CCEDAEDFC6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B7BE6A-2B1B-4C65-8BFE-73D06C1C0C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4815" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="4440" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Promotion" sheetId="1" r:id="rId1"/>
+    <sheet name="Email List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="221">
   <si>
     <t>Product name</t>
   </si>
@@ -677,6 +678,12 @@
   </si>
   <si>
     <t>LTT</t>
+  </si>
+  <si>
+    <t>Guy Dixon, &lt;guydixon@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Mark McCorkle, &lt;mccorkle@devteam.org&gt;</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4838,4 +4845,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC47473-D2F1-454E-BEF6-5721D896EFF9}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>